<commit_message>
add Venu for PO_Framework project, optimize for other framework
</commit_message>
<xml_diff>
--- a/SeleniumPythonFramework/src/TestScript/Module2/LaunchBaiduAndSearch1/Search1.xlsx
+++ b/SeleniumPythonFramework/src/TestScript/Module2/LaunchBaiduAndSearch1/Search1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8016" windowWidth="14808" xWindow="240" yWindow="108"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -80,18 +80,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -394,17 +394,17 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="3" width="17.6640625"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="3" width="8.88671875"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" style="3" width="12.6640625"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="3" width="21.5546875"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" style="3" width="9.6640625"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" style="3" width="13.44140625"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="3" width="13.109375"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" style="3" width="6.5546875"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" style="3" width="4"/>
-    <col customWidth="1" max="10" min="10" style="3" width="8.88671875"/>
-    <col customWidth="1" max="16384" min="11" style="3" width="8.88671875"/>
+    <col width="17.6640625" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
+    <col width="8.88671875" bestFit="1" customWidth="1" style="3" min="2" max="2"/>
+    <col width="12.6640625" bestFit="1" customWidth="1" style="3" min="3" max="3"/>
+    <col width="21.5546875" bestFit="1" customWidth="1" style="3" min="4" max="4"/>
+    <col width="9.6640625" bestFit="1" customWidth="1" style="3" min="5" max="5"/>
+    <col width="13.44140625" bestFit="1" customWidth="1" style="3" min="6" max="6"/>
+    <col width="13.109375" bestFit="1" customWidth="1" style="3" min="7" max="7"/>
+    <col width="6.5546875" bestFit="1" customWidth="1" style="3" min="8" max="8"/>
+    <col width="4" bestFit="1" customWidth="1" style="3" min="9" max="9"/>
+    <col width="8.88671875" customWidth="1" style="3" min="10" max="10"/>
+    <col width="8.88671875" customWidth="1" style="3" min="11" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -487,7 +487,7 @@
       </c>
       <c r="G2" s="3" t="inlineStr">
         <is>
-          <t>0130_215757.png</t>
+          <t>0606_091803.png</t>
         </is>
       </c>
       <c r="H2" s="3" t="inlineStr">
@@ -497,7 +497,7 @@
       </c>
       <c r="I2" s="3" t="inlineStr">
         <is>
-          <t>01-30 21:57:57 setText execution was Passed</t>
+          <t>06-06 09:18:03 setText execution was Passed</t>
         </is>
       </c>
     </row>
@@ -534,7 +534,7 @@
       </c>
       <c r="G3" s="3" t="inlineStr">
         <is>
-          <t>0130_215758.png</t>
+          <t>0606_091804.png</t>
         </is>
       </c>
       <c r="H3" s="3" t="inlineStr">
@@ -544,12 +544,12 @@
       </c>
       <c r="I3" s="3" t="inlineStr">
         <is>
-          <t>01-30 21:57:58 click execution was Passed</t>
+          <t>06-06 09:18:04 click execution was Passed</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
@@ -568,7 +568,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -586,6 +586,6 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>